<commit_message>
more knowledge about pcl
</commit_message>
<xml_diff>
--- a/Team-Building/SkillSetAnalysis.xlsx
+++ b/Team-Building/SkillSetAnalysis.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Luca/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -151,6 +159,12 @@
   </si>
   <si>
     <t>Experience in data science (analysis/treatment/processing/modelling)</t>
+  </si>
+  <si>
+    <t>Have experience with research, could do sketches in documentation</t>
+  </si>
+  <si>
+    <t>Worked in real software building environment and managed a startup of about 12 collegues as co founder</t>
   </si>
 </sst>
 </file>
@@ -227,7 +241,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -303,12 +317,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -350,12 +367,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -385,12 +402,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -596,28 +613,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.42578125"/>
-    <col min="2" max="2" width="20.28515625"/>
-    <col min="3" max="3" width="8.42578125"/>
-    <col min="4" max="4" width="19.5703125"/>
-    <col min="5" max="5" width="8.42578125"/>
-    <col min="6" max="6" width="11.28515625"/>
-    <col min="7" max="7" width="27.85546875"/>
-    <col min="8" max="8" width="9.28515625"/>
-    <col min="9" max="9" width="14.5703125"/>
-    <col min="10" max="10" width="37.5703125"/>
-    <col min="11" max="11" width="8.42578125"/>
-    <col min="12" max="12" width="15.28515625"/>
-    <col min="13" max="1025" width="8.42578125"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,7 +651,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -659,18 +661,30 @@
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="L2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="120" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>42</v>
       </c>
@@ -705,7 +719,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -726,7 +740,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="105" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -761,7 +775,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="180" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -793,7 +807,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -811,7 +825,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
@@ -843,7 +857,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -861,7 +875,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="195" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>34</v>
       </c>
@@ -872,26 +886,28 @@
         <v>36</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J10" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="135" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
@@ -901,15 +917,29 @@
       <c r="C11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="75" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>

</xml_diff>